<commit_message>
Add descriptions on important lines.
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigrp17\Documents\CS161\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigrp17\Documents\laserficheprogrammingproblemsolvingexercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42,7 +42,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,12 +50,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,212 +355,291 @@
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection sqref="A1:W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-      <c r="I1">
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
         <v>7</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="1">
         <v>8</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="1">
         <v>9</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="1">
         <v>10</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="1">
         <v>11</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="1">
         <v>12</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="1">
         <v>13</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="1">
         <v>14</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="1">
         <v>15</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="1">
         <v>16</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="1">
         <v>17</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="1">
         <v>18</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="1">
         <v>19</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="1">
         <v>20</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1">
         <v>7</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>8</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>9</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>11</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>12</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <v>13</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="1">
         <v>14</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="1">
         <v>15</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="1">
         <v>16</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="1">
         <v>17</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="1">
         <v>18</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="1">
         <v>19</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="1">
         <v>20</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>4</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1">
+        <v>6</v>
+      </c>
+      <c r="O3" s="1">
+        <v>7</v>
+      </c>
+      <c r="P3" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>3</v>
+      </c>
+      <c r="R3" s="1">
+        <v>4</v>
+      </c>
+      <c r="S3" s="1">
+        <v>5</v>
+      </c>
+      <c r="T3" s="1">
+        <v>6</v>
+      </c>
+      <c r="U3" s="1">
+        <v>7</v>
+      </c>
+      <c r="V3" s="1">
+        <v>8</v>
+      </c>
+      <c r="W3" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1">
+        <v>3</v>
+      </c>
+      <c r="L4" s="1">
+        <v>4</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1">
+        <v>6</v>
+      </c>
+      <c r="O4" s="1">
+        <v>7</v>
+      </c>
+      <c r="P4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>3</v>
+      </c>
+      <c r="T4" s="1">
+        <v>4</v>
+      </c>
+      <c r="U4" s="1">
+        <v>5</v>
+      </c>
+      <c r="V4" s="1">
+        <v>6</v>
+      </c>
+      <c r="W4" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>